<commit_message>
xoa cac phan tong cua ti le chiet khau
</commit_message>
<xml_diff>
--- a/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
+++ b/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V72"/>
+  <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6496,51 +6496,137 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>07-25-2024</t>
+        </is>
+      </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>590</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Trần Thị Lệ</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Phạm Thanh Hoàng</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="J72" t="n">
+        <v/>
+      </c>
+      <c r="K72" t="n">
+        <v/>
+      </c>
+      <c r="L72" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Phạm Thanh Hoàng</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v/>
+      </c>
+      <c r="O72" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="T72" t="n">
+        <v/>
+      </c>
+      <c r="U72" t="n">
+        <v>100000</v>
+      </c>
+      <c r="V72" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="C72" t="n">
-        <v>70</v>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="n">
-        <v>480268000</v>
-      </c>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="n">
+      <c r="C73" t="n">
+        <v>71</v>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="n">
+        <v>499268000</v>
+      </c>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="n">
         <v>26000000</v>
       </c>
-      <c r="L72" t="n">
-        <v>506268000</v>
-      </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="n">
-        <v>449968000</v>
-      </c>
-      <c r="P72" t="n">
+      <c r="L73" t="n">
+        <v>525268000</v>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="n">
+        <v>468968000</v>
+      </c>
+      <c r="P73" t="n">
         <v>22500000</v>
       </c>
-      <c r="Q72" t="n">
-        <v>472468000</v>
-      </c>
-      <c r="R72" t="n">
+      <c r="Q73" t="n">
+        <v>491468000</v>
+      </c>
+      <c r="R73" t="n">
         <v>33800000</v>
       </c>
-      <c r="S72" t="inlineStr"/>
-      <c r="T72" t="inlineStr"/>
-      <c r="U72" t="n">
-        <v>2850000</v>
-      </c>
-      <c r="V72" t="n">
-        <v>550000</v>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="n">
+        <v>2950000</v>
+      </c>
+      <c r="V73" t="n">
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
@@ -6554,7 +6640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10033,17 +10119,73 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>703</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>07-25-2024</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>LONG XUYÊN</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Ứng Lương</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>704</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>07-25-2024</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>LONG XUYÊN</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Chi Phí CTV</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B125" t="n">
-        <v>123</v>
-      </c>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr"/>
-      <c r="F125" t="n">
-        <v>267881000</v>
+      <c r="B127" t="n">
+        <v>125</v>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="n">
+        <v>269931000</v>
       </c>
     </row>
   </sheetData>
@@ -10189,7 +10331,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30970000</v>
+        <v>31520000</v>
       </c>
     </row>
     <row r="3">
@@ -10269,7 +10411,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>45689000</v>
+        <v>47189000</v>
       </c>
     </row>
     <row r="11">
@@ -10289,7 +10431,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>267881000</v>
+        <v>269931000</v>
       </c>
     </row>
   </sheetData>
@@ -10303,7 +10445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10926,26 +11068,51 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>07-25-2024</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="C25" t="n">
+        <v>19000000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3500000</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2050000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>20450000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>506268000</v>
-      </c>
-      <c r="C25" t="n">
-        <v>449968000</v>
-      </c>
-      <c r="D25" t="n">
-        <v>70</v>
-      </c>
-      <c r="E25" t="n">
-        <v>74500000</v>
-      </c>
-      <c r="F25" t="n">
-        <v>267881000</v>
-      </c>
-      <c r="G25" t="n">
-        <v>256587000</v>
+      <c r="B26" t="n">
+        <v>525268000</v>
+      </c>
+      <c r="C26" t="n">
+        <v>468968000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>71</v>
+      </c>
+      <c r="E26" t="n">
+        <v>78000000</v>
+      </c>
+      <c r="F26" t="n">
+        <v>269931000</v>
+      </c>
+      <c r="G26" t="n">
+        <v>277037000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code for KPI update
</commit_message>
<xml_diff>
--- a/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
+++ b/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
@@ -10199,7 +10199,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10210,7 +10210,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Mã nhân viên</t>
+          <t>Nhân viên</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -10262,34 +10262,714 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Bác Sĩ Ngoài</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7800000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bác Sĩ Thảo</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>38000000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CTV Ngoài</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4500000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kha Như Huỳnh </t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2400000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>800000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4288000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" t="n">
+        <v>700000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La Thị Ngọc Hà My </t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10688000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>96700000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>73600000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lê Hoàng Thanh</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Lê Văn Linh</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>27000000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lê Đình Hậu</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>118000000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9000000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoàng Yến Quyên</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>9600000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2300000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>132400000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Nguyễn Phúc Nam</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>28850000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Phạm Thanh Hoàng</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>67000000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>195730000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sang sang</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Thạch Hoàng Nhân</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>66000000</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Trương Lâm Khanh</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2600000</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Trần Khánh Hiệp</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Đào Vương Anh</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" t="n">
+        <v>250000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Đặng Ngọc Mai</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>21650000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>50330000</v>
+      </c>
+      <c r="C21" t="n">
+        <v>13900000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="B22" t="n">
+        <v>488768000</v>
+      </c>
+      <c r="C22" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>473468000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>32</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update code tinh luong
</commit_message>
<xml_diff>
--- a/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
+++ b/Báo cáo/0_HỆ THỐNG/HỆ THỐNG 2024-07-01 - 2024-07-30.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6050,21 +6050,23 @@
         <v>22000000</v>
       </c>
       <c r="P66" t="n">
-        <v>0</v>
+        <v>7000000</v>
       </c>
       <c r="Q66" t="n">
-        <v>22000000</v>
+        <v>29000000</v>
       </c>
       <c r="R66" t="n">
-        <v>7000000</v>
+        <v>0</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
           <t xml:space="preserve">Kha Như Huỳnh </t>
         </is>
       </c>
-      <c r="T66" t="n">
-        <v/>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>Trần Khánh Hiệp</t>
+        </is>
       </c>
       <c r="U66" t="n">
         <v>100000</v>
@@ -6104,7 +6106,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Khách cũ</t>
+          <t>Cá nhân</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -6582,51 +6584,637 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>07-26-2024</t>
+        </is>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>591</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Cắt mí</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Huỳnh Huyền Trân</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="J73" t="n">
+        <v/>
+      </c>
+      <c r="K73" t="n">
+        <v/>
+      </c>
+      <c r="L73" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoàng Yến Quyên</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v/>
+      </c>
+      <c r="O73" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="R73" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="T73" t="n">
+        <v/>
+      </c>
+      <c r="U73" t="n">
+        <v>50000</v>
+      </c>
+      <c r="V73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>593</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trần thị ngọc bích </t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>15000000</v>
+      </c>
+      <c r="J74" t="n">
+        <v/>
+      </c>
+      <c r="K74" t="n">
+        <v/>
+      </c>
+      <c r="L74" t="n">
+        <v>15000000</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v/>
+      </c>
+      <c r="O74" t="n">
+        <v>15000000</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>15000000</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kha Như Huỳnh </t>
+        </is>
+      </c>
+      <c r="T74" t="n">
+        <v/>
+      </c>
+      <c r="U74" t="n">
+        <v>100000</v>
+      </c>
+      <c r="V74" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>594</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>thạch thị sơ ri</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Thạch Hoàng Nhân</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>35000000</v>
+      </c>
+      <c r="J75" t="n">
+        <v/>
+      </c>
+      <c r="K75" t="n">
+        <v/>
+      </c>
+      <c r="L75" t="n">
+        <v>35000000</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v/>
+      </c>
+      <c r="O75" t="n">
+        <v>35000000</v>
+      </c>
+      <c r="P75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>35000000</v>
+      </c>
+      <c r="R75" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kha Như Huỳnh </t>
+        </is>
+      </c>
+      <c r="T75" t="n">
+        <v/>
+      </c>
+      <c r="U75" t="n">
+        <v>100000</v>
+      </c>
+      <c r="V75" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>595</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trương thị lan </t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="J76" t="n">
+        <v/>
+      </c>
+      <c r="K76" t="n">
+        <v/>
+      </c>
+      <c r="L76" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>Phạm Thanh Hoàng</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v/>
+      </c>
+      <c r="O76" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="R76" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="T76" t="n">
+        <v/>
+      </c>
+      <c r="U76" t="n">
+        <v>100000</v>
+      </c>
+      <c r="V76" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>596</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Cắt mí</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>bảo trân</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Lê Đình Hậu</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="J77" t="n">
+        <v/>
+      </c>
+      <c r="K77" t="n">
+        <v/>
+      </c>
+      <c r="L77" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoàng Yến Quyên</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v/>
+      </c>
+      <c r="O77" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="R77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>Trần Khánh Hiệp</t>
+        </is>
+      </c>
+      <c r="T77" t="n">
+        <v/>
+      </c>
+      <c r="U77" t="n">
+        <v>50000</v>
+      </c>
+      <c r="V77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>597</v>
+      </c>
+      <c r="D78" t="n">
+        <v/>
+      </c>
+      <c r="E78" t="n">
+        <v/>
+      </c>
+      <c r="F78" t="n">
+        <v/>
+      </c>
+      <c r="G78" t="n">
+        <v/>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v/>
+      </c>
+      <c r="J78" t="n">
+        <v/>
+      </c>
+      <c r="K78" t="n">
+        <v/>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="n">
+        <v/>
+      </c>
+      <c r="N78" t="n">
+        <v/>
+      </c>
+      <c r="O78" t="n">
+        <v/>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="n">
+        <v/>
+      </c>
+      <c r="T78" t="n">
+        <v/>
+      </c>
+      <c r="U78" t="n">
+        <v/>
+      </c>
+      <c r="V78" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>598</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Cọc Dịch Vụ Làm Đẹp</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Thị Minh</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Lê Hoàng Thanh</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>200000</v>
+      </c>
+      <c r="J79" t="n">
+        <v/>
+      </c>
+      <c r="K79" t="n">
+        <v/>
+      </c>
+      <c r="L79" t="n">
+        <v>200000</v>
+      </c>
+      <c r="M79" t="n">
+        <v/>
+      </c>
+      <c r="N79" t="n">
+        <v/>
+      </c>
+      <c r="O79" t="n">
+        <v>200000</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>200000</v>
+      </c>
+      <c r="R79" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="n">
+        <v/>
+      </c>
+      <c r="T79" t="n">
+        <v/>
+      </c>
+      <c r="U79" t="n">
+        <v/>
+      </c>
+      <c r="V79" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="C73" t="n">
-        <v>71</v>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="n">
-        <v>499268000</v>
-      </c>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="n">
+      <c r="C80" t="n">
+        <v>78</v>
+      </c>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="n">
+        <v>575468000</v>
+      </c>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="n">
         <v>26000000</v>
       </c>
-      <c r="L73" t="n">
-        <v>525268000</v>
-      </c>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
-      <c r="O73" t="n">
-        <v>468968000</v>
-      </c>
-      <c r="P73" t="n">
-        <v>22500000</v>
-      </c>
-      <c r="Q73" t="n">
-        <v>491468000</v>
-      </c>
-      <c r="R73" t="n">
-        <v>33800000</v>
-      </c>
-      <c r="S73" t="inlineStr"/>
-      <c r="T73" t="inlineStr"/>
-      <c r="U73" t="n">
-        <v>2950000</v>
-      </c>
-      <c r="V73" t="n">
-        <v>600000</v>
+      <c r="L80" t="n">
+        <v>601468000</v>
+      </c>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="n">
+        <v>545168000</v>
+      </c>
+      <c r="P80" t="n">
+        <v>29500000</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>574668000</v>
+      </c>
+      <c r="R80" t="n">
+        <v>26800000</v>
+      </c>
+      <c r="S80" t="inlineStr"/>
+      <c r="T80" t="inlineStr"/>
+      <c r="U80" t="n">
+        <v>3350000</v>
+      </c>
+      <c r="V80" t="n">
+        <v>750000</v>
       </c>
     </row>
   </sheetData>
@@ -6640,7 +7228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10175,17 +10763,241 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>705</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>LONG XUYÊN</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Trang thiết bị Y Tế</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>58000</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>706</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>LONG XUYÊN</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Chi Phí Sinh Hoạt Tại Cơ Sở</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>176000</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>707</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Ứng Lương</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>708</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Ứng Lương</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>709</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Chi Phí Sinh Hoạt Tại Cơ Sở</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>715000</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>710</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Chi Phí Vận Hành</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>711</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Trang thiết bị Y Tế</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>712</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Chi Phí CTV</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B127" t="n">
-        <v>125</v>
-      </c>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr"/>
-      <c r="F127" t="n">
-        <v>269931000</v>
+      <c r="B135" t="n">
+        <v>133</v>
+      </c>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="n">
+        <v>286580000</v>
       </c>
     </row>
   </sheetData>
@@ -10380,10 +11192,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>700000</v>
+        <v>900000</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -10448,10 +11260,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>1050000</v>
+        <v>1200000</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -10470,13 +11282,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>96700000</v>
+        <v>129700000</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>73600000</v>
+        <v>130600000</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -10504,7 +11316,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1800000</v>
+        <v>2000000</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -10572,7 +11384,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>118000000</v>
+        <v>120000000</v>
       </c>
       <c r="C11" t="n">
         <v>9000000</v>
@@ -10612,7 +11424,7 @@
         <v>2300000</v>
       </c>
       <c r="D12" t="n">
-        <v>132400000</v>
+        <v>140400000</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -10680,7 +11492,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>195730000</v>
+        <v>213730000</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -10742,7 +11554,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>66000000</v>
+        <v>101000000</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -10822,16 +11634,16 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -10912,7 +11724,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>50330000</v>
+        <v>56330000</v>
       </c>
       <c r="C21" t="n">
         <v>13900000</v>
@@ -10946,28 +11758,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>488768000</v>
+        <v>564968000</v>
       </c>
       <c r="C22" t="n">
         <v>26000000</v>
       </c>
       <c r="D22" t="n">
-        <v>473468000</v>
+        <v>556468000</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G22" t="n">
-        <v>2100000</v>
+        <v>2500000</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" t="n">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -11011,7 +11823,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31520000</v>
+        <v>38520000</v>
       </c>
     </row>
     <row r="3">
@@ -11031,7 +11843,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11777000</v>
+        <v>12668000</v>
       </c>
     </row>
     <row r="5">
@@ -11041,7 +11853,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18540000</v>
+        <v>18840000</v>
       </c>
     </row>
     <row r="6">
@@ -11081,7 +11893,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17863000</v>
+        <v>20321000</v>
       </c>
     </row>
     <row r="10">
@@ -11091,7 +11903,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>47189000</v>
+        <v>53189000</v>
       </c>
     </row>
     <row r="11">
@@ -11111,7 +11923,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>269931000</v>
+        <v>286580000</v>
       </c>
     </row>
   </sheetData>
@@ -11125,7 +11937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11773,26 +12585,76 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>07-26-2024</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="C26" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>07-28-2024</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>70200000</v>
+      </c>
+      <c r="C27" t="n">
+        <v>70200000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7000000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>16649000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>60551000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>525268000</v>
-      </c>
-      <c r="C26" t="n">
-        <v>468968000</v>
-      </c>
-      <c r="D26" t="n">
-        <v>71</v>
-      </c>
-      <c r="E26" t="n">
-        <v>78000000</v>
-      </c>
-      <c r="F26" t="n">
-        <v>269931000</v>
-      </c>
-      <c r="G26" t="n">
-        <v>277037000</v>
+      <c r="B28" t="n">
+        <v>601468000</v>
+      </c>
+      <c r="C28" t="n">
+        <v>545168000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>78</v>
+      </c>
+      <c r="E28" t="n">
+        <v>85000000</v>
+      </c>
+      <c r="F28" t="n">
+        <v>286580000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>343588000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>